<commit_message>
service assignment and view done
</commit_message>
<xml_diff>
--- a/public/individual.xlsx
+++ b/public/individual.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SSN</t>
   </si>
@@ -36,9 +36,6 @@
     <t>ZIP_CODE</t>
   </si>
   <si>
-    <t>SERVICE_NAME</t>
-  </si>
-  <si>
     <t>FIRST_NAME</t>
   </si>
   <si>
@@ -54,10 +51,10 @@
     <t>EMAIL_ADDRESS</t>
   </si>
   <si>
-    <t>DATA_OF_BIRTH</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>DATE_OF_BIRTH</t>
   </si>
 </sst>
 </file>
@@ -342,78 +339,81 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K13" s="3"/>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
individual leads import done
</commit_message>
<xml_diff>
--- a/public/individual.xlsx
+++ b/public/individual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PROJECTS\LARAVEL\CRM_roles_permision\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SSN</t>
   </si>
@@ -36,9 +36,6 @@
     <t>ZIP_CODE</t>
   </si>
   <si>
-    <t>SERVICE_NAME</t>
-  </si>
-  <si>
     <t>FIRST_NAME</t>
   </si>
   <si>
@@ -54,10 +51,10 @@
     <t>EMAIL_ADDRESS</t>
   </si>
   <si>
-    <t>DATA_OF_BIRTH</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>DATE_OF_BIRTH</t>
   </si>
 </sst>
 </file>
@@ -342,78 +339,75 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K13" s="3"/>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>